<commit_message>
Modified process to allow for initial automation. Refactoring needed.
</commit_message>
<xml_diff>
--- a/docs/tracking_metric_definitions.xlsx
+++ b/docs/tracking_metric_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AElborolosy/Projects/ref_tracking_metrics/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3D513F-87CE-B643-A321-81F027D499A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D328F2E-CE72-CA42-9F3C-D3CDA7BB18B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EC9E95FA-937D-534C-A947-A45E0E32813E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{EC9E95FA-937D-534C-A947-A45E0E32813E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Trail Possessions Quit</t>
+  </si>
+  <si>
+    <t>Optimal</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Less</t>
   </si>
 </sst>
 </file>
@@ -478,9 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB1B5B3-D22E-0942-8EAB-881CBCF658A3}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -488,7 +499,7 @@
     <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,10 +513,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -519,10 +533,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -536,10 +553,13 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -553,10 +573,13 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -570,10 +593,13 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -587,10 +613,13 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -604,10 +633,13 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -621,6 +653,9 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flagging errors and viewing them
</commit_message>
<xml_diff>
--- a/docs/tracking_metric_definitions.xlsx
+++ b/docs/tracking_metric_definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AElborolosy/Projects/ref_tracking_metrics/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AElborolosy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D328F2E-CE72-CA42-9F3C-D3CDA7BB18B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1D885D-60BD-5C48-85AE-D6EAD345CE91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{EC9E95FA-937D-534C-A947-A45E0E32813E}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{EC9E95FA-937D-534C-A947-A45E0E32813E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -57,45 +57,15 @@
     <t>Lead</t>
   </si>
   <si>
-    <t>avg_dist_lead_basket</t>
-  </si>
-  <si>
-    <t>Lead Distance on Shooting Fouls</t>
-  </si>
-  <si>
-    <t>Time to Baseline</t>
-  </si>
-  <si>
-    <t>time_to_baseline</t>
-  </si>
-  <si>
     <t>Transition</t>
   </si>
   <si>
-    <t>Average distance from basket when calling shooting fouls</t>
-  </si>
-  <si>
-    <t>perc_time_near_ft_line</t>
-  </si>
-  <si>
     <t>Slot</t>
   </si>
   <si>
-    <t>Time it takes the lead ref to get to the baseline from the other side of the court</t>
-  </si>
-  <si>
-    <t>Distance from Pack</t>
-  </si>
-  <si>
     <t>Time near FT Line Extended</t>
   </si>
   <si>
-    <t>Distance Slot ref is from the middle of the pack extended</t>
-  </si>
-  <si>
-    <t>distance_from_pack</t>
-  </si>
-  <si>
     <t>Trail</t>
   </si>
   <si>
@@ -108,27 +78,12 @@
     <t>% of time spent at least 3 feet behind the basketball in transition</t>
   </si>
   <si>
-    <t>perc_time_in_position_halfcourt</t>
-  </si>
-  <si>
-    <t>perc_time_in_position_transition</t>
-  </si>
-  <si>
     <t>Trail behind ball - Transition</t>
   </si>
   <si>
     <t>Trail behind ball - Halfcourt</t>
   </si>
   <si>
-    <t>% of possessions where the trail starts transitioning before the end of possessions</t>
-  </si>
-  <si>
-    <t>perc_poss_quit</t>
-  </si>
-  <si>
-    <t>Trail Possessions Quit</t>
-  </si>
-  <si>
     <t>Optimal</t>
   </si>
   <si>
@@ -136,6 +91,54 @@
   </si>
   <si>
     <t>Less</t>
+  </si>
+  <si>
+    <t>transition_speed</t>
+  </si>
+  <si>
+    <t>Trail to Lead</t>
+  </si>
+  <si>
+    <t>Speed at which the lead ref gets to the baseline from the other side of the court at the start of a possession</t>
+  </si>
+  <si>
+    <t>Trail Stay on Play</t>
+  </si>
+  <si>
+    <t>perc_poss_completed/shifted</t>
+  </si>
+  <si>
+    <t>% of possessions where the trail does not transition until the possession is completed</t>
+  </si>
+  <si>
+    <t>perc_time_near_ft_line_ext</t>
+  </si>
+  <si>
+    <t>More/Undefined</t>
+  </si>
+  <si>
+    <t>perc_time_behind_ball_halfcourt</t>
+  </si>
+  <si>
+    <t>Trail by 28 Foot Mark</t>
+  </si>
+  <si>
+    <t>perc_time_by_28_mark</t>
+  </si>
+  <si>
+    <t>Base Lead</t>
+  </si>
+  <si>
+    <t>perc_time_in_base_position_lead</t>
+  </si>
+  <si>
+    <t>% of time spent at least 12 feet out of the rim.</t>
+  </si>
+  <si>
+    <t>% of time spent at least 3 feet of the 28 Foot Mark</t>
+  </si>
+  <si>
+    <t>perc_time_behind_ball_transition</t>
   </si>
 </sst>
 </file>
@@ -489,14 +492,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB1B5B3-D22E-0942-8EAB-881CBCF658A3}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -513,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -521,22 +526,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -544,99 +549,99 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -644,19 +649,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>